<commit_message>
CDS test cases updates
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_FileType-BAI.xlsx
+++ b/InputFiles/TC01_CDS_Filter_FileType-BAI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B018B4C2-7EB6-4F2F-B792-56AAEFD97301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C6CC25-FAE4-4D56-95AC-8BE1A7C47FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
CDS Input file updates
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_FileType-BAI.xlsx
+++ b/InputFiles/TC01_CDS_Filter_FileType-BAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C6CC25-FAE4-4D56-95AC-8BE1A7C47FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A61651-2B71-48C6-9D7E-BC540320C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -104,19 +104,24 @@
 ORDER By f.file_name LIMIT 100</t>
   </si>
   <si>
-    <t>MATCH (f:file)
+    <t>MATCH (p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH s, p, samp, f, g, diag
 WHERE f.file_type in ['BAI']
-MATCH (f)--&gt;(:sample)--&gt;(p:participant)--&gt;(s:study)
-MATCH (samp:sample)--&gt;(p)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN 
-    coalesce(p.participant_id,'') as `Participant ID`,
-    coalesce(s.study_name, '') as `Study Name`,
-    coalesce(s.phs_accession,'') as `Accession`,
-    coalesce(p.gender,'') as `Gender`,
-    coalesce(apoc.text.join(samp, ','), '') as `Samples`
-ORDER BY `Participant ID`
-LIMIT 100</t>
+with p
+OPTIONAL MATCH (p)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
+RETURN
+coalesce(p.participant_id,'') as `Participant ID`,
+coalesce(s.study_name, '') as `Study Name`,
+coalesce(s.phs_accession,'') as `Accession`,
+coalesce(p.gender,'') as `Gender`,
+coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ORDER BY p.participant_id LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -527,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="201.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="279" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>